<commit_message>
adjusting and adding excel files, adding a new api
</commit_message>
<xml_diff>
--- a/members-information.xlsx
+++ b/members-information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training Rony\web0\GP\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6499C5-5C3E-4EB4-8C40-7D4A2F9A5E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0106A012-DDD3-4E85-A5C2-9D8A1BC7F706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,25 +48,25 @@
     <t>Peter Nguyen</t>
   </si>
   <si>
-    <t>CEO: As the CEO of Powerful Digital Solutions, John is responsible for the overall strategic direction of the company and ensuring that it continues to provide top-notch digital solutions to its clients.</t>
-  </si>
-  <si>
-    <t>Director of Development: Alex manages the development team at Powerful Digital Solutions, ensuring that all website and app projects are completed on time and to the highest quality standards.</t>
-  </si>
-  <si>
-    <t>Analytics Specialist: David specializes in analytics and reporting, helping clients track and analyze the performance of their digital marketing campaigns and make data-driven decisions for future strategies.</t>
-  </si>
-  <si>
-    <t>Director of Marketing: Sarah oversees all of the marketing efforts at Powerful Digital Solutions, including SEO, PPC, social media, content creation, and email marketing.</t>
-  </si>
-  <si>
-    <t>Content Manager: Emily is in charge of all content creation and marketing efforts at Powerful Digital Solutions, working closely with clients to develop engaging and relevant content for their target audiences.</t>
-  </si>
-  <si>
-    <t>Creative Director: Maria oversees all creative design efforts at Powerful Digital Solutions, ensuring that each project meets the specific needs and vision of the client while adhering to best practices in design.</t>
-  </si>
-  <si>
-    <t>Project Manager: Peter is responsible for managing all client projects at Powerful Digital Solutions, working closely with the development, marketing, and creative teams to ensure that each project is completed on time, within budget, and to the client's satisfaction.</t>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>Director of Marketing</t>
+  </si>
+  <si>
+    <t>Director of Development</t>
+  </si>
+  <si>
+    <t>Content Manager</t>
+  </si>
+  <si>
+    <t>Analytics Specialist</t>
+  </si>
+  <si>
+    <t>Creative Director</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
   </si>
 </sst>
 </file>
@@ -408,7 +408,7 @@
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="242.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -430,7 +430,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -441,7 +441,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -452,7 +452,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -463,7 +463,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>